<commit_message>
ya no incluye bajas automaticas
</commit_message>
<xml_diff>
--- a/NRFM_Auditoria/NRFM_Auditoria/bin/Debug/net8.0-windows/Extracciones/4-2024/DIEGO ALDANA.xlsx
+++ b/NRFM_Auditoria/NRFM_Auditoria/bin/Debug/net8.0-windows/Extracciones/4-2024/DIEGO ALDANA.xlsx
@@ -68,31 +68,31 @@
     <x:t>Comentarios</x:t>
   </x:si>
   <x:si>
+    <x:t>LUEVANO DE LEON LEONARDO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NRLLL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ACTIVO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>QualityOffer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>X385058</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DIEGO ALDANA</x:t>
+  </x:si>
+  <x:si>
     <x:t>ARMENDARIZ ADRIANA GUADAL</x:t>
   </x:si>
   <x:si>
     <x:t>NRAAG2</x:t>
   </x:si>
   <x:si>
-    <x:t>ACTIVO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>QualityOffer</x:t>
-  </x:si>
-  <x:si>
     <x:t>ArmendA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DIEGO ALDANA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LUEVANO DE LEON LEONARDO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NRLLL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>X385058</x:t>
   </x:si>
   <x:si>
     <x:t>IAPI</x:t>
@@ -248,7 +248,7 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="5">
+  <x:cellStyleXfs count="6">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -264,8 +264,11 @@
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="22" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="5">
+  <x:cellXfs count="6">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -283,6 +286,10 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -672,10 +679,10 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="F6" s="4">
-        <x:v>45139</x:v>
-      </x:c>
-      <x:c r="G6" s="4">
-        <x:v>45349</x:v>
+        <x:v>43122</x:v>
+      </x:c>
+      <x:c r="G6" s="5">
+        <x:v>45306.5833217593</x:v>
       </x:c>
       <x:c r="H6" s="3" t="s">
         <x:v>19</x:v>
@@ -703,10 +710,10 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="F7" s="4">
-        <x:v>43122</x:v>
-      </x:c>
-      <x:c r="G7" s="4">
-        <x:v>45349</x:v>
+        <x:v>45139</x:v>
+      </x:c>
+      <x:c r="G7" s="5">
+        <x:v>45323.7184606481</x:v>
       </x:c>
       <x:c r="H7" s="3" t="s">
         <x:v>23</x:v>
@@ -868,7 +875,7 @@
         <x:v>33</x:v>
       </x:c>
       <x:c r="C9" s="3" t="s">
-        <x:v>23</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D9" s="3" t="s">
         <x:v>27</x:v>
@@ -987,7 +994,7 @@
         <x:v>44757</x:v>
       </x:c>
       <x:c r="G6" s="4">
-        <x:v>45341</x:v>
+        <x:v>45330</x:v>
       </x:c>
       <x:c r="H6" s="3" t="s">
         <x:v>20</x:v>
@@ -1015,7 +1022,7 @@
         <x:v>44757</x:v>
       </x:c>
       <x:c r="G7" s="4">
-        <x:v>45348</x:v>
+        <x:v>45334</x:v>
       </x:c>
       <x:c r="H7" s="3" t="s">
         <x:v>20</x:v>
@@ -1043,7 +1050,7 @@
         <x:v>44757</x:v>
       </x:c>
       <x:c r="G8" s="4">
-        <x:v>45355</x:v>
+        <x:v>45307</x:v>
       </x:c>
       <x:c r="H8" s="3" t="s">
         <x:v>20</x:v>
@@ -1071,7 +1078,7 @@
         <x:v>44757</x:v>
       </x:c>
       <x:c r="G9" s="4">
-        <x:v>45337</x:v>
+        <x:v>45322</x:v>
       </x:c>
       <x:c r="H9" s="3" t="s">
         <x:v>20</x:v>
@@ -1099,7 +1106,7 @@
         <x:v>44757</x:v>
       </x:c>
       <x:c r="G10" s="4">
-        <x:v>45345</x:v>
+        <x:v>45334</x:v>
       </x:c>
       <x:c r="H10" s="3" t="s">
         <x:v>20</x:v>

</xml_diff>